<commit_message>
add wiz note loader
</commit_message>
<xml_diff>
--- a/yaoapp/data/test.xlsx
+++ b/yaoapp/data/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\go\yao\wwsheng009\yao-plugin-document-loader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\go\yao\wwsheng009\yao-plugin-document-loader\yaoapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0171D157-D095-48B4-87FB-2BA41CCD58EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B955293A-D7B0-4130-93A6-339A3D1850C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="27936" windowHeight="13824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="27936" windowHeight="13824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" activeCellId="1" sqref="A2:B21 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -392,7 +392,178 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">NOW()</f>
-        <v>45295.942333796294</v>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>124</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B21" ca="1" si="0">NOW()</f>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>125</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>126</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>127</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>129</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>130</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>131</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>132</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>133</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>134</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>135</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>136</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>137</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>138</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>139</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>140</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>141</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>142</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45296.008931944445</v>
       </c>
     </row>
   </sheetData>
@@ -403,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A09EAC2-F6C5-47CF-9C9A-EC5FB1708906}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -428,7 +599,55 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">NOW()</f>
-        <v>45295.942333796294</v>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4790</v>
+      </c>
+      <c r="B3" s="1">
+        <f ca="1">NOW()</f>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4791</v>
+      </c>
+      <c r="B4" s="1">
+        <f ca="1">NOW()</f>
+        <v>45296.008931944445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4796</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>